<commit_message>
Timing for Matrix Factorization
</commit_message>
<xml_diff>
--- a/python-code/graphing/timing.xlsx
+++ b/python-code/graphing/timing.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet name="user_based" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="item_based" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Matrix_Factorization" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -12,15 +13,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Runtime</t>
+    <t>Best Runtime</t>
   </si>
   <si>
-    <t>11-12-2018</t>
+    <t>Average Runtime</t>
+  </si>
+  <si>
+    <t>11-13-2018</t>
   </si>
 </sst>
 </file>
@@ -28,15 +32,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="m/d/yy" numFmtId="164"/>
+    <numFmt formatCode="m-d-yyyy" numFmtId="164"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Arial"/>
       <color rgb="FF000000"/>
       <sz val="10"/>
     </font>
     <font/>
+    <font>
+      <name val="Arial"/>
+      <color rgb="FF000000"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -64,12 +72,19 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -366,31 +381,50 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="3" min="1" style="5" width="18.57"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2" t="n"/>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="n">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="n">
+        <v>43415</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>1.59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="n">
+        <v>43416</v>
+      </c>
+      <c r="B3" s="4" t="n">
         <v>1.58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1.54</v>
       </c>
     </row>
   </sheetData>
@@ -404,31 +438,99 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="3" min="1" style="5" width="18.57"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2" t="n"/>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="n">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="n">
+        <v>43415</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>4.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="n">
+        <v>43416</v>
+      </c>
+      <c r="B3" s="4" t="n">
         <v>4.57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>4.53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="3" min="1" style="5" width="18.57"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="n">
+        <v>43415</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>1.59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="n">
+        <v>43416</v>
+      </c>
+      <c r="B3" s="4" t="n">
+        <v>1.58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed corrupted xlsx file
</commit_message>
<xml_diff>
--- a/python-code/graphing/timing.xlsx
+++ b/python-code/graphing/timing.xlsx
@@ -5,7 +5,6 @@
   <sheets>
     <sheet name="user_based" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="item_based" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Matrix_Factorization" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,10 +17,10 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Best Runtime</t>
+    <t>Runtime</t>
   </si>
   <si>
-    <t>Average Runtime</t>
+    <t>11-12-2018</t>
   </si>
   <si>
     <t>11-13-2018</t>
@@ -32,19 +31,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="m-d-yyyy" numFmtId="164"/>
+    <numFmt formatCode="m/d/yy" numFmtId="164"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Arial"/>
       <color rgb="FF000000"/>
       <sz val="10"/>
     </font>
     <font/>
-    <font>
-      <name val="Arial"/>
-      <color rgb="FF000000"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -72,19 +67,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -381,50 +369,39 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75" outlineLevelCol="0"/>
-  <cols>
-    <col customWidth="1" max="3" min="1" style="5" width="18.57"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="n"/>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2" t="n">
-        <v>43415</v>
-      </c>
-      <c r="B2" s="3" t="n">
-        <v>1.59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2" t="n">
-        <v>43416</v>
-      </c>
-      <c r="B3" s="4" t="n">
+      <c r="B3" t="n">
         <v>1.58</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>1.54</v>
+        <v>1.53</v>
       </c>
     </row>
   </sheetData>
@@ -438,99 +415,39 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75" outlineLevelCol="0"/>
-  <cols>
-    <col customWidth="1" max="3" min="1" style="5" width="18.57"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="n"/>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2" t="n">
-        <v>43415</v>
-      </c>
-      <c r="B2" s="3" t="n">
-        <v>4.6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2" t="n">
-        <v>43416</v>
-      </c>
-      <c r="B3" s="4" t="n">
+      <c r="B3" t="n">
         <v>4.57</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>4.53</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75" outlineLevelCol="0"/>
-  <cols>
-    <col customWidth="1" max="3" min="1" style="5" width="18.57"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2" t="n">
-        <v>43415</v>
-      </c>
-      <c r="B2" s="3" t="n">
-        <v>1.59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2" t="n">
-        <v>43416</v>
-      </c>
-      <c r="B3" s="4" t="n">
-        <v>1.58</v>
+        <v>4.56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>